<commit_message>
Excel import for Zabbix
</commit_message>
<xml_diff>
--- a/hostlist.xlsx
+++ b/hostlist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Firma_Adi</t>
   </si>
@@ -44,6 +44,54 @@
   </si>
   <si>
     <t xml:space="preserve">Polling Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Istanbul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisco Catalyst 29xxStack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.20.30.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ankara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Router</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juniper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juniper EX3300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.40.50.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICMP</t>
   </si>
 </sst>
 </file>
@@ -90,36 +138,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF729FCF"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,28 +180,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -194,66 +206,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF729FCF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF81D41A"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -265,10 +217,10 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.62"/>
@@ -292,21 +244,73 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
+      <c r="B10" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>